<commit_message>
Updates per Lisa's feedback
</commit_message>
<xml_diff>
--- a/output/observations-summary.xlsx
+++ b/output/observations-summary.xlsx
@@ -59,7 +59,7 @@
     <t/>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-codes (example)</t>
+    <t>http://example.org/ValueSet/SymptomsVS (preferred)</t>
   </si>
   <si>
     <t>dateTime, Period, Timing, instant</t>
@@ -74,7 +74,7 @@
     <t>optional</t>
   </si>
   <si>
-    <t>CodeableConcept, Ratio</t>
+    <t>Quantity, CodeableConcept, Ratio</t>
   </si>
   <si>
     <t>CodeableConcept, string</t>

</xml_diff>